<commit_message>
added the gigignore file and also added the prediction for next day entry and exit point
</commit_message>
<xml_diff>
--- a/Data/My History.xlsx
+++ b/Data/My History.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heman\Desktop\stockMarket\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heman\Desktop\stockMarket\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713FE7E6-A82C-4571-9549-FF454188803E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E577883-4F92-428E-AFD4-10B0331E88F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -76,6 +76,24 @@
   </si>
   <si>
     <t xml:space="preserve">Avilable Quantity </t>
+  </si>
+  <si>
+    <t>IRCON</t>
+  </si>
+  <si>
+    <t>29-01-2024</t>
+  </si>
+  <si>
+    <t>ELECTCAST</t>
+  </si>
+  <si>
+    <t>NHPC</t>
+  </si>
+  <si>
+    <t>Loss</t>
+  </si>
+  <si>
+    <t>SUZLON</t>
   </si>
 </sst>
 </file>
@@ -117,8 +135,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,7 +441,7 @@
     <col min="12" max="12" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,19 +478,22 @@
       <c r="L1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C2">
-        <v>410</v>
+        <v>247.25</v>
       </c>
       <c r="D2">
-        <v>420.25</v>
+        <v>238.8</v>
       </c>
       <c r="E2">
         <v>20</v>
@@ -478,9 +501,6 @@
       <c r="F2">
         <v>20</v>
       </c>
-      <c r="G2">
-        <v>205</v>
-      </c>
       <c r="K2" t="s">
         <v>6</v>
       </c>
@@ -488,32 +508,185 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>410</v>
+      </c>
+      <c r="D3">
+        <v>420.25</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+      <c r="G3">
+        <v>205</v>
+      </c>
+      <c r="K3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>4462.7</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>4439</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <v>1</v>
       </c>
-      <c r="F3">
+      <c r="F4">
         <v>1</v>
       </c>
-      <c r="G3">
+      <c r="G4">
         <v>23.7</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K4" t="s">
         <v>14</v>
       </c>
-      <c r="L3">
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>45293</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>420.75</v>
+      </c>
+      <c r="E5">
+        <v>40</v>
+      </c>
+      <c r="K5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>45293</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>171.35</v>
+      </c>
+      <c r="D6">
+        <v>177</v>
+      </c>
+      <c r="E6">
+        <v>19</v>
+      </c>
+      <c r="F6">
+        <v>19</v>
+      </c>
+      <c r="K6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>45293</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>90.5</v>
+      </c>
+      <c r="D7">
+        <v>97</v>
+      </c>
+      <c r="E7">
+        <v>40</v>
+      </c>
+      <c r="F7">
+        <v>40</v>
+      </c>
+      <c r="K7" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>45324</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>4291.2</v>
+      </c>
+      <c r="D8">
+        <v>4312.75</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>-21.55</v>
+      </c>
+      <c r="K8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>45324</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9">
+        <v>48.9</v>
+      </c>
+      <c r="E9">
+        <v>90</v>
+      </c>
+      <c r="K9" t="s">
+        <v>6</v>
+      </c>
+      <c r="L9">
         <v>0</v>
       </c>
     </row>

</xml_diff>